<commit_message>
making process data files
</commit_message>
<xml_diff>
--- a/input_files/Inputs.xlsx
+++ b/input_files/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\alpha-pilot-champs\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED8F02C-9C59-4FD8-9A93-58E72E15938C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BAA5D8-BA5C-4598-914E-3BFD1B1B2179}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="1272" windowWidth="17280" windowHeight="8964" xr2:uid="{F952EA37-474F-44BC-902B-9398AE2F677A}"/>
+    <workbookView xWindow="3156" yWindow="1620" windowWidth="17280" windowHeight="8964" xr2:uid="{F952EA37-474F-44BC-902B-9398AE2F677A}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,7 +417,7 @@
         <v>5</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -425,7 +425,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -437,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4812C92A-6A87-400C-A90B-D4CBD1CB5B56}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Some updates to costFunction and inequalities
</commit_message>
<xml_diff>
--- a/input_files/Inputs.xlsx
+++ b/input_files/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\alpha-pilot-champs\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CB2551-D365-49B8-A7A9-A118D514A648}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C05349-7132-42A6-A370-920058937544}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24855" yWindow="4065" windowWidth="17280" windowHeight="8970" xr2:uid="{F952EA37-474F-44BC-902B-9398AE2F677A}"/>
+    <workbookView xWindow="-19035" yWindow="4920" windowWidth="17280" windowHeight="8970" xr2:uid="{F952EA37-474F-44BC-902B-9398AE2F677A}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,7 +417,7 @@
         <v>5</v>
       </c>
       <c r="B1">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -425,7 +425,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4812C92A-6A87-400C-A90B-D4CBD1CB5B56}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>